<commit_message>
Revert to git reset --soft HEAD@{1}
</commit_message>
<xml_diff>
--- a/media/test_imports/sample_contacts.xlsx
+++ b/media/test_imports/sample_contacts.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/norbert/nyaruka/rapidpro/media/test_imports/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C852B35-E133-6A44-9D88-42E405919FEE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="460" windowWidth="25600" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2680" yWindow="0" windowWidth="25600" windowHeight="18180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Table 1 - Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="4294967295"/>
+  <calcPr calcId="4294967295" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,6 +30,9 @@
     <t>Eric Newcomer</t>
   </si>
   <si>
+    <t>phone</t>
+  </si>
+  <si>
     <t>jen newcomer</t>
   </si>
   <si>
@@ -43,15 +40,12 @@
   </si>
   <si>
     <t>250(78) 8 383 383</t>
-  </si>
-  <si>
-    <t>URN:Tel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,14 +159,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -482,7 +468,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -526,7 +512,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -547,29 +533,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IU4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="255" width="10.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="255" width="10.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>250788382382</v>
       </c>
@@ -577,20 +565,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="4" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>